<commit_message>
corrections of the definitions
</commit_message>
<xml_diff>
--- a/EDA/Hanwash_new_Indicators.xlsx
+++ b/EDA/Hanwash_new_Indicators.xlsx
@@ -627,7 +627,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>This indicator measures the level of engagement and support provided by Rotarians in WASH-related events in local communes, reflecting increased civil society engagement in WASH services.</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -636,13 +636,13 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="J4" t="n">
         <v>100</v>
       </c>
       <c r="K4" t="n">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5">
@@ -676,7 +676,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>…led by Rotarians… means the WASH activities whose initiative have been taken by Rotarians.</t>
+          <t>The percentage of WASH events within communes that are led and coordinated by trained HANWASH Ambassadors and Coordinators, aiming to effectively communicate WASH messages and advocate for HANWASH goals. This reflects the level of leadership and initiative taken by trained personnel in promoting WASH activities.</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -685,13 +685,13 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="J5" t="n">
         <v>100</v>
       </c>
       <c r="K5" t="n">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6">
@@ -723,20 +723,24 @@
           <t># of volunteer hours per month spent by Rotarians in WASH events</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>The total number of hours that Rotarians volunteer each month participating in WASH initiatives and activities.</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr">
         <is>
           <t>volunteer hours / club / month</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J6" t="n">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="K6" t="n">
-        <v>15</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7">
@@ -770,7 +774,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Number of people reached…: Number of people participating in the WASH events led by Rotarians.</t>
+          <t>The total number of individuals who participate in or are impacted by WASH events and advocacy efforts led by HANWASH Ambassadors, Coordinators, and Rotarians. This indicates the outreach and engagement success of the WASH programs.</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -779,13 +783,13 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="J7" t="n">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="K7" t="n">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
@@ -819,7 +823,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>The total number of HANWASH Ambassadors who have successfully completed their training programs.</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -828,13 +832,13 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="J8" t="n">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="K8" t="n">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9">
@@ -868,7 +872,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>The total number of HANWASH Coordinators who have successfully completed their training programs.</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -877,13 +881,13 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="J9" t="n">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="K9" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
@@ -917,7 +921,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>-</t>
+          <t xml:space="preserve"> The total count of educational and training materials developed that adhere to the three pillars and core values of HANWASH.</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -926,13 +930,13 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="J10" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K10" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -975,13 +979,13 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="J11" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="K11" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -1015,7 +1019,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>...in alignment with Commune Action Plans:-The activity was originally a part of a commune action plan, then implemented as part of a HANWASH project.</t>
+          <t xml:space="preserve"> The percentage of WASH interventions that have been approved and implemented in accordance with predefined Commune Action Plans, ensuring the initiatives are part of a strategic and coordinated approach to WASH improvements.</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1024,13 +1028,13 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="J12" t="n">
         <v>100</v>
       </c>
       <c r="K12" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13">
@@ -1064,7 +1068,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>The number of communes that have developed action plans explicitly addressing water, sanitation, hygiene, and water resources management.</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1073,13 +1077,13 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K13" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1113,7 +1117,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>The number of meetings and events held to plan and coordinate WASH activities involving DINEPA and municipal officials.</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1125,10 +1129,10 @@
         <v>1</v>
       </c>
       <c r="J14" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1162,7 +1166,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>National guidelines:-Water points: 1 x water survey per year-Piped water systems: 1 x Monthly Report per month</t>
+          <t xml:space="preserve"> The percentage of service providers participating in the HANWASH initiative that are regularly monitored according to established national guidelines. This metric ensures that WASH service providers meet accountability standards, maintain quality service delivery, and uphold their responsibilities towards users as per national regulatory requirements.</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1171,13 +1175,13 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="J15" t="n">
         <v>100</v>
       </c>
       <c r="K15" t="n">
-        <v>78</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16">
@@ -1211,7 +1215,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Accountability structures in place:) Committee meets regularly) Committee meets with community regularly) Committee bylaws in place) Fees are collected) Records are available; 6) Reports are submitted to OREPA and the local authorities on a monthly basis</t>
+          <t>The percentage of service providers with established accountability mechanisms, such as regular meetings, community engagement, bylaws, fee collection, record-keeping, and monthly reporting to local authorities.</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1220,13 +1224,13 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="J16" t="n">
         <v>100</v>
       </c>
       <c r="K16" t="n">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17">
@@ -1269,13 +1273,13 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>69</v>
+        <v>32</v>
       </c>
       <c r="J17" t="n">
         <v>100</v>
       </c>
       <c r="K17" t="n">
-        <v>74</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18">
@@ -1309,7 +1313,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Regularly reporting data:) Submitted their monthly report</t>
+          <t>The number of water systems within intervention areas that consistently submit monthly operational and performance reports, ensuring regular monitoring and transparency of water service delivery.</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1358,7 +1362,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Percent of complaints: 100 x # of complaints resolved during the month  # of complaints identified during the month</t>
+          <t xml:space="preserve"> The percentage of customer complaints that are resolved within the same month they are identified.</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1367,13 +1371,13 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="J19" t="n">
         <v>100</v>
       </c>
       <c r="K19" t="n">
-        <v>71</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20">
@@ -1416,13 +1420,13 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J20" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="K20" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -1509,7 +1513,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Functioning:a) Functional: Water point is in good working condition and regularly provides water according the specifications in the original design.ORb) Partially functional but in need of repair: Water point provides water on a regular basis (possibly in a reduced capacity) but repairs are needed due to some maintece issue or change in conditions at the site.Potable: ) Free from E. Coli and priority contamits</t>
+          <t>The percentage of water points in intervention areas that are operational (either fully functional or functional with minor repairs needed) and provide potable water, free from E. Coli and other priority contaminants, according to original design specifications.</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1518,13 +1522,13 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J22" t="n">
         <v>100</v>
       </c>
       <c r="K22" t="n">
-        <v>81</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
@@ -1558,7 +1562,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>...at least basic drinking water service:) Improved water source) Within 30 min round tripNote: This also includes basic and safely managed water service.</t>
+          <t>The percentage of people in intervention communes who have access to an improved water source within a 30-minute round trip, ensuring basic drinking water service at the household level.</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1567,13 +1571,13 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="J23" t="n">
         <v>100</v>
       </c>
       <c r="K23" t="n">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24">
@@ -1607,7 +1611,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Safely managed drinking water service:) Improved water source) Accessible on premises) Available when needed) Free from E. Coli and priority contamits</t>
+          <t>The percentage of people in target areas who have access to safe drinking water that is always available, accessible at home, and free from contaminants.</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1616,13 +1620,13 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="J24" t="n">
         <v>100</v>
       </c>
       <c r="K24" t="n">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25">
@@ -1656,7 +1660,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>1a) Functional: Water point is in good working condition and regularly provides water according the specifications in the original design.ORb) Partially functional but in need of repair: Water point provides water on a regular basis (possibly in a reduced capacity) but repairs are needed due to some maintece issue or change in conditions at the site.) Potable: Free from E. Coli and priority contamits.) have a balanced budget:Monthly revenue excceeds expenses.) after 2 years: Two years from the inauguration date.</t>
+          <t>The percentage of water points in intervention areas that are fully operational, provide potable water, and maintain a balanced or surplus budget within two years from their inauguration date.</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1665,13 +1669,13 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>85</v>
+        <v>47</v>
       </c>
       <c r="J25" t="n">
         <v>100</v>
       </c>
       <c r="K25" t="n">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26">
@@ -1705,7 +1709,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Basic drinking water service:) Improved water source) Within 30 min round trip) [Household level]</t>
+          <t>The number of individuals in intervention communes who benefit from access to basic drinking water services provided by community-managed water points, ensuring sustainable and locally-managed water supply solutions.</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1714,13 +1718,13 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="J26" t="n">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="K26" t="n">
-        <v>49</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27">
@@ -1754,7 +1758,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Community managed water points:) Signed CPE statutes with DINEPA</t>
+          <t>The total number of water points established and managed by local communities under DINEPA's guidelines.</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1763,13 +1767,13 @@
         </is>
       </c>
       <c r="I27" t="n">
+        <v>35</v>
+      </c>
+      <c r="J27" t="n">
+        <v>185</v>
+      </c>
+      <c r="K27" t="n">
         <v>72</v>
-      </c>
-      <c r="J27" t="n">
-        <v>175</v>
-      </c>
-      <c r="K27" t="n">
-        <v>118</v>
       </c>
     </row>
     <row r="28">
@@ -1803,7 +1807,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Community managed water points:) Signed CPE statutes with DINEPA</t>
+          <t>The percentage of community-managed water points that submit monthly reports to local authorities.</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1812,13 +1816,13 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>160</v>
+        <v>70</v>
       </c>
       <c r="J28" t="n">
-        <v>193</v>
+        <v>164</v>
       </c>
       <c r="K28" t="n">
-        <v>174</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29">
@@ -1852,7 +1856,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Safely managed drinking water service:) Improved water source) Available on premises) Available when needed) Free from E. Coli and priority contamits</t>
+          <t>The number of individuals who have gained access to safe drinking water through the project.</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1861,10 +1865,10 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="J29" t="n">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="K29" t="n">
         <v>66</v>
@@ -1901,7 +1905,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Professionally managed water systems:) Signed OP statutes with DINEPA; Rehabilitated means: The term rehabilitated implies that there was a pre-existing water supply system that may have been damaged, degraded, or in need of upgrades, and efforts were made to restore or enhance its functionality.</t>
+          <t>The number of existing piped water systems that have been restored to proper functionality in the target areas.</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1913,10 +1917,10 @@
         <v>1</v>
       </c>
       <c r="J30" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1950,7 +1954,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Professionally managed water systems:) Signed OP statutes with DINEPA</t>
+          <t>The number of new piped water systems established and professionally managed in the target areas.</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1999,7 +2003,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Verified ODF:) [Verification conducted by commune WASH committee]) 100% of households have a toilet that has been used at least once) Toilets meet the minimum standards of hygiene, privacy, and security) Areas of defecation identified during contact visits, reported no evidence of fecal matter) Schools attended by 80% of children comply with health standards) Main market frequented by the population has a usable sanitary block or a formal step has been undertaken for this purpose) There is a willingness of the locality to maintain a state of ODF</t>
+          <t>The percentage of communities in intervention areas that have been verified as Open Defecation Free by the commune WASH committee, meeting criteria such as the presence of usable toilets, no fecal matter in open areas, and willingness to maintain ODF status.</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2008,13 +2012,13 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="J32" t="n">
         <v>100</v>
       </c>
       <c r="K32" t="n">
-        <v>69</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33">
@@ -2048,7 +2052,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>...at least basic sanitation service: Basic) Improved) Unshared) [Household level]Note: Includes basic and safely managed sanitation service.</t>
+          <t xml:space="preserve"> The percentage of people in intervention communes who have access to improved and unshared sanitation facilities, ensuring basic sanitation service at the household level.</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2057,13 +2061,13 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="J33" t="n">
         <v>100</v>
       </c>
       <c r="K33" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34">
@@ -2097,7 +2101,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Safely managed sanitation service:) Improved) UnsharedANDa) Excretia treated in situ ORb) Excretia emptied, transported, and treated</t>
+          <t>The percentage of people in target areas who have access to safe, private (unshared) sanitation facilities where excreta are properly treated on-site or transported and treated off-site.</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2106,13 +2110,13 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="J34" t="n">
         <v>100</v>
       </c>
       <c r="K34" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35">
@@ -2146,7 +2150,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Basic sanitation service:) Improved) Unshared) [Household level]</t>
+          <t>The number of individuals newly provided with access to basic sanitation services, including improved and unshared facilities, within intervention communes.</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2155,13 +2159,13 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="J35" t="n">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="K35" t="n">
-        <v>52</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36">
@@ -2195,7 +2199,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Verified ODF:) [Verification conducted by commune WASH committee]) 100% of households have a toilet that has been used at least once) Toilets meet the minimum standards of hygiene, privacy, and security) Areas of defecation identified during contact visits, reported no evidence of fecal matter) Schools attended by 80% of children comply with health standards) Main market frequented by the population has a usable sanitary block or a formal step has been undertaken for this purpose) There is a willingness of the locality to maintain a state of ODF</t>
+          <t>The total number of communities in intervention areas that have achieved verification as Open Defecation Free, meeting the criteria set by the commune WASH committee.</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2204,13 +2208,13 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>106</v>
+        <v>21</v>
       </c>
       <c r="J36" t="n">
-        <v>126</v>
+        <v>140</v>
       </c>
       <c r="K36" t="n">
-        <v>118</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37">
@@ -2244,7 +2248,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Certified ODF:) [Certification conducted by commune WASH committee]) Maintained Verified ODF criteria (see below) for at least 1 year.Verified ODF:) [Verification conducted by commune WASH committee]) 100% of households have a toilet that has been used at least once) Toilets meet the minimum standards of hygiene, privacy, and security) Areas of defecation identified during contact visits, reported no evidence of fecal matter) Schools attended by 80% of children comply with health standards) Main market frequented by the population has a usable sanitary block or a formal step has been undertaken for this purpose) There is a willingness of the locality to maintain a state of ODF</t>
+          <t>The number of communities in intervention areas that have sustained Open Defecation Free status for at least one year and have been officially certified by the commune WASH committee.</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2253,13 +2257,13 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J37" t="n">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="K37" t="n">
-        <v>91</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38">
@@ -2293,7 +2297,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>The number of public latrines built within the project scope.</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2302,13 +2306,13 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>101</v>
+        <v>9</v>
       </c>
       <c r="J38" t="n">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="K38" t="n">
-        <v>103</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39">
@@ -2342,7 +2346,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>...at least basic hygiene service:) Presence of a Hanwashing facility on premises) Presence of soap and water</t>
+          <t>The percentage of people in intervention communes who have access to facilities with soap and water for handwashing, ensuring basic hygiene service at the household level.</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2351,13 +2355,13 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>95</v>
+        <v>20</v>
       </c>
       <c r="J39" t="n">
         <v>100</v>
       </c>
       <c r="K39" t="n">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40">
@@ -2391,7 +2395,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Basic hygiene service:) Presence of a Hanwashing facility on premises) Presence of soap and water</t>
+          <t>The percentage of individuals newly provided with access to basic hygiene services, including handwashing facilities with soap and water within intervention communes.</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2400,13 +2404,13 @@
         </is>
       </c>
       <c r="I40" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="J40" t="n">
         <v>100</v>
       </c>
       <c r="K40" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41">
@@ -2440,7 +2444,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>The total number of community animators who have completed training programs.</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2449,13 +2453,13 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="J41" t="n">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="K41" t="n">
-        <v>49</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42">
@@ -2498,13 +2502,13 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="J42" t="n">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="K42" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43">
@@ -2538,7 +2542,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Basic hygiene service:) Presence of a facility) Presence of soap and water) [Household level]</t>
+          <t>The number of individuals newly provided with access to basic hygiene services, including handwashing facilities with soap and water within intervention communes.</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2547,13 +2551,13 @@
         </is>
       </c>
       <c r="I43" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="J43" t="n">
-        <v>83</v>
+        <v>46</v>
       </c>
       <c r="K43" t="n">
-        <v>60</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44">
@@ -2587,7 +2591,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Basic drinking water service:) Improved) Currently availableBasic sanitation service:) Improved) Usable) Single sex toilets availableBasic hygiene service:) Presence of handwashing facilities) Presence of soap and water</t>
+          <t>The percentage of schools in intervention areas that have improved, safe drinking water sources, functional sanitation facilities, and handwashing stations with soap and water.</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2596,13 +2600,13 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="J44" t="n">
         <v>100</v>
       </c>
       <c r="K44" t="n">
-        <v>93</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45">
@@ -2636,7 +2640,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Basic drinking water service:) Improved) On premises) Currently availableBasic sanitation service:) Improved) Usable) Dedicated for staff) Sex-separated with menstrual hygiene facilities) Accessible for users with limited mobilityBasic hygiene service:...At points of care) Facilities present) Soap and water or alcohol based hand rub present...At toilets) Within 5 m of toilets) Facilities present) Soap and water present</t>
+          <t>The percentage of healthcare facilities in intervention areas that have improved, safe drinking water sources, functioning sanitation facilities, and handwashing stations with soap and water or alcohol-based hand rubs. This metric ensures that healthcare facilities meet basic WASH standards.</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2645,13 +2649,13 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="J45" t="n">
         <v>100</v>
       </c>
       <c r="K45" t="n">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46">
@@ -2685,7 +2689,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Basic drinking water service:) Improved) Currently available</t>
+          <t>The total number of schools in intervention areas that have been provided with access to improved drinking water services, ensuring that they meet the required standards of water quality and availability.</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2694,13 +2698,13 @@
         </is>
       </c>
       <c r="I46" t="n">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="J46" t="n">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="K46" t="n">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47">
@@ -2734,7 +2738,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Basic drinking water service:) Improved) On premises) Currently available</t>
+          <t>The total number of healthcare facilities in intervention areas that have been provided with access to improved drinking water services, ensuring safe and reliable water for patients and staff.</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2743,13 +2747,13 @@
         </is>
       </c>
       <c r="I47" t="n">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="J47" t="n">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K47" t="n">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48">
@@ -2783,7 +2787,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Basic sanitation service:) Improved) Usable) Single sex toilets available</t>
+          <t>The total number of schools in intervention areas that have been equipped with improved, functional sanitation facilities, including gender-separated and accessible toilets, to meet the needs of students and staff.</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2792,13 +2796,13 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>37</v>
+        <v>116</v>
       </c>
       <c r="J48" t="n">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="K48" t="n">
-        <v>108</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49">
@@ -2832,7 +2836,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Basic sanitation services:) Improved) Usable) Dedicated for staff) Sex-separated with menstrual hygiene facilities) Accessible for users with limited mobility</t>
+          <t>The total number of healthcare facilities in intervention areas that have been equipped with improved, functional sanitation facilities, including dedicated and accessible toilets. These facilities are designed to meet the sanitation needs of all healthcare users.</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2841,13 +2845,13 @@
         </is>
       </c>
       <c r="I49" t="n">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="J49" t="n">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="K49" t="n">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50">
@@ -2881,7 +2885,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Basic hygiene:) Presence of handwashing facilities) Presence of soap and water</t>
+          <t>The total number of schools in intervention areas that have been provided with handwashing facilities, including soap and water, ensuring basic hygiene practices are accessible to all students and staff.</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2890,13 +2894,13 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>56</v>
+        <v>169</v>
       </c>
       <c r="J50" t="n">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="K50" t="n">
-        <v>161</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51">
@@ -2930,7 +2934,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Basic hygiene:...At points of care) Facilities present) Soap and water or alcohol based hand rub present...At toilets) Within 5 m of toilets) Facilities present) Soap and water present</t>
+          <t>The total number of healthcare facilities in intervention areas that have been provided with handwashing facilities, including soap and water or alcohol-based hand rubs, ensuring basic hygiene practices are accessible to all patients and staff.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2939,13 +2943,13 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>127</v>
+        <v>14</v>
       </c>
       <c r="J51" t="n">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="K51" t="n">
-        <v>160</v>
+        <v>97</v>
       </c>
     </row>
     <row r="52">
@@ -3032,7 +3036,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Aligned with HANWASH Core Values:-### **LOCALLY LED****We strengthen community participation in goverce of WASH infrastructure and services.**### **COLLABORATIVE****Volunteers, government authorities, and partners are meaningfully engaged.**### ****### **SYSTEMATIC****We will be thoughtful and consistent in planning, doing, and improving our work.**### **IMPACTFUL****Sustainability is a key metric of our success.******### **COMMITTED****We will not stop until the job is done.**</t>
+          <t>The total amount of funds pledged by stakeholders in accordance with HANWASH Core Values.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -3041,13 +3045,13 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>2244</v>
+        <v>646</v>
       </c>
       <c r="J53" t="n">
-        <v>14085</v>
+        <v>10675</v>
       </c>
       <c r="K53" t="n">
-        <v>11744</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="54">
@@ -3081,7 +3085,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>% spent (cumulative): (Cumulative_amount_spent  Cumulative_amount_committed) x 100</t>
+          <t>The cumulative percentage of allocated funds that have been spent over the project duration. This metric is calculated by dividing the total amount spent by the total committed funds and multiplying by 100, reflecting the financial resource utilization efficiency of the project.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -3090,13 +3094,13 @@
         </is>
       </c>
       <c r="I54" t="n">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="J54" t="n">
         <v>100</v>
       </c>
       <c r="K54" t="n">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55">
@@ -3130,7 +3134,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Aligned with HANWASH Core Values:-### **LOCALLY LED****We strengthen community participation in goverce of WASH infrastructure and services.**### **COLLABORATIVE****Volunteers, government authorities, and partners are meaningfully engaged.**### ****### **SYSTEMATIC****We will be thoughtful and consistent in planning, doing, and improving our work.**### **IMPACTFUL****Sustainability is a key metric of our success.******### **COMMITTED****We will not stop until the job is done.**</t>
+          <t>The total amount of money spent by external organizations or entities within the areas covered by HANWASH projects.</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -3139,13 +3143,13 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>7267</v>
+        <v>5376</v>
       </c>
       <c r="J55" t="n">
-        <v>14590</v>
+        <v>5669</v>
       </c>
       <c r="K55" t="n">
-        <v>11915</v>
+        <v>5525</v>
       </c>
     </row>
     <row r="56">
@@ -3179,7 +3183,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Aligned with HANWASH Core Values:-### **LOCALLY LED****We strengthen community participation in goverce of WASH infrastructure and services.**### **COLLABORATIVE****Volunteers, government authorities, and partners are meaningfully engaged.**### ****### **SYSTEMATIC****We will be thoughtful and consistent in planning, doing, and improving our work.**### **IMPACTFUL****Sustainability is a key metric of our success.******### **COMMITTED****We will not stop until the job is done.**</t>
+          <t>The total amount of money spent by external entities outside the HANWASH project areas, in line with HANWASH Core Values.</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -3188,13 +3192,13 @@
         </is>
       </c>
       <c r="I56" t="n">
-        <v>1085</v>
+        <v>7859</v>
       </c>
       <c r="J56" t="n">
-        <v>1915</v>
+        <v>15348</v>
       </c>
       <c r="K56" t="n">
-        <v>1876</v>
+        <v>13865</v>
       </c>
     </row>
     <row r="57">
@@ -3237,13 +3241,13 @@
         </is>
       </c>
       <c r="I57" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J57" t="n">
         <v>100</v>
       </c>
       <c r="K57" t="n">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58">
@@ -3277,7 +3281,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>The total number of DINEPA personnel who have undergone leadership training programs.</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3286,13 +3290,13 @@
         </is>
       </c>
       <c r="I58" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="J58" t="n">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="K58" t="n">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59">
@@ -3326,7 +3330,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Priorities areas for 2023-24: Unified national tariff methodology &amp; ODF certification.</t>
+          <t>The number of technical training sessions delivered to address DINEPA's prioritized areas, including the unified national tariff methodology and ODF certification for 2023-24.</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -3335,13 +3339,13 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J59" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="K59" t="n">
-        <v>21</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new structure for the progression table
</commit_message>
<xml_diff>
--- a/EDA/Hanwash_new_Indicators.xlsx
+++ b/EDA/Hanwash_new_Indicators.xlsx
@@ -496,7 +496,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -549,7 +549,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -604,7 +604,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -636,13 +636,13 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="J4" t="n">
         <v>100</v>
       </c>
       <c r="K4" t="n">
-        <v>65</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -685,13 +685,13 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="J5" t="n">
         <v>100</v>
       </c>
       <c r="K5" t="n">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6">
@@ -702,7 +702,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -734,13 +734,13 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="J6" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K6" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
@@ -751,7 +751,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -783,13 +783,13 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="J7" t="n">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="K7" t="n">
-        <v>21</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
@@ -800,7 +800,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -832,13 +832,13 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="J8" t="n">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="K8" t="n">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
@@ -849,7 +849,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -881,13 +881,13 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="J9" t="n">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="K9" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
@@ -898,7 +898,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -930,13 +930,13 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="J10" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K10" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11">
@@ -947,7 +947,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -979,13 +979,13 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J11" t="n">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="K11" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
@@ -996,7 +996,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1028,13 +1028,13 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="J12" t="n">
         <v>100</v>
       </c>
       <c r="K12" t="n">
-        <v>98</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13">
@@ -1045,7 +1045,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1080,10 +1080,10 @@
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -1094,7 +1094,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1126,13 +1126,13 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1175,13 +1175,13 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="J15" t="n">
         <v>100</v>
       </c>
       <c r="K15" t="n">
-        <v>37</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1224,13 +1224,13 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="J16" t="n">
         <v>100</v>
       </c>
       <c r="K16" t="n">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1273,13 +1273,13 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="J17" t="n">
         <v>100</v>
       </c>
       <c r="K17" t="n">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18">
@@ -1290,7 +1290,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1322,13 +1322,13 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1339,7 +1339,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1371,13 +1371,13 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="J19" t="n">
         <v>100</v>
       </c>
       <c r="K19" t="n">
-        <v>97</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1420,13 +1420,13 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J20" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="K20" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1490,7 +1490,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1522,13 +1522,13 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="J22" t="n">
         <v>100</v>
       </c>
       <c r="K22" t="n">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1571,13 +1571,13 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="J23" t="n">
         <v>100</v>
       </c>
       <c r="K23" t="n">
-        <v>74</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24">
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1620,13 +1620,13 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="J24" t="n">
         <v>100</v>
       </c>
       <c r="K24" t="n">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25">
@@ -1637,7 +1637,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1669,13 +1669,13 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="J25" t="n">
         <v>100</v>
       </c>
       <c r="K25" t="n">
-        <v>93</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26">
@@ -1686,7 +1686,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1718,13 +1718,13 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="J26" t="n">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="K26" t="n">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27">
@@ -1735,7 +1735,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1767,13 +1767,13 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="J27" t="n">
-        <v>185</v>
+        <v>108</v>
       </c>
       <c r="K27" t="n">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28">
@@ -1784,7 +1784,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1816,13 +1816,13 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>70</v>
+        <v>119</v>
       </c>
       <c r="J28" t="n">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="K28" t="n">
-        <v>113</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29">
@@ -1833,7 +1833,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1865,13 +1865,13 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="J29" t="n">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="K29" t="n">
-        <v>66</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1917,10 +1917,10 @@
         <v>1</v>
       </c>
       <c r="J30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1980,7 +1980,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2012,13 +2012,13 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="J32" t="n">
         <v>100</v>
       </c>
       <c r="K32" t="n">
-        <v>97</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2061,13 +2061,13 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="J33" t="n">
         <v>100</v>
       </c>
       <c r="K33" t="n">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2110,13 +2110,13 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="J34" t="n">
         <v>100</v>
       </c>
       <c r="K34" t="n">
-        <v>81</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35">
@@ -2127,7 +2127,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -2159,13 +2159,13 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="J35" t="n">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="K35" t="n">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -2208,10 +2208,10 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="J36" t="n">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="K36" t="n">
         <v>125</v>
@@ -2225,7 +2225,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2257,13 +2257,13 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="J37" t="n">
-        <v>133</v>
+        <v>104</v>
       </c>
       <c r="K37" t="n">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2306,13 +2306,13 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="J38" t="n">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="K38" t="n">
-        <v>43</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -2355,13 +2355,13 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="J39" t="n">
         <v>100</v>
       </c>
       <c r="K39" t="n">
-        <v>95</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40">
@@ -2372,7 +2372,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -2404,13 +2404,13 @@
         </is>
       </c>
       <c r="I40" t="n">
-        <v>98</v>
+        <v>32</v>
       </c>
       <c r="J40" t="n">
         <v>100</v>
       </c>
       <c r="K40" t="n">
-        <v>99</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -2453,13 +2453,13 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="J41" t="n">
         <v>95</v>
       </c>
       <c r="K41" t="n">
-        <v>90</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42">
@@ -2470,7 +2470,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -2505,10 +2505,10 @@
         <v>14</v>
       </c>
       <c r="J42" t="n">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="K42" t="n">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43">
@@ -2519,7 +2519,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -2551,13 +2551,13 @@
         </is>
       </c>
       <c r="I43" t="n">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="J43" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K43" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -2600,13 +2600,13 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="J44" t="n">
         <v>100</v>
       </c>
       <c r="K44" t="n">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45">
@@ -2617,7 +2617,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2649,13 +2649,13 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>81</v>
+        <v>29</v>
       </c>
       <c r="J45" t="n">
         <v>100</v>
       </c>
       <c r="K45" t="n">
-        <v>88</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46">
@@ -2666,7 +2666,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -2698,13 +2698,13 @@
         </is>
       </c>
       <c r="I46" t="n">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="J46" t="n">
-        <v>168</v>
+        <v>124</v>
       </c>
       <c r="K46" t="n">
-        <v>148</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47">
@@ -2715,7 +2715,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -2747,13 +2747,13 @@
         </is>
       </c>
       <c r="I47" t="n">
-        <v>175</v>
+        <v>2</v>
       </c>
       <c r="J47" t="n">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="K47" t="n">
-        <v>176</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48">
@@ -2764,7 +2764,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2796,13 +2796,13 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="J48" t="n">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="K48" t="n">
-        <v>131</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -2845,13 +2845,13 @@
         </is>
       </c>
       <c r="I49" t="n">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="J49" t="n">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="K49" t="n">
-        <v>133</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50">
@@ -2862,7 +2862,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2894,13 +2894,13 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>169</v>
+        <v>98</v>
       </c>
       <c r="J50" t="n">
-        <v>194</v>
+        <v>151</v>
       </c>
       <c r="K50" t="n">
-        <v>192</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51">
@@ -2911,7 +2911,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2943,13 +2943,13 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="J51" t="n">
-        <v>105</v>
+        <v>157</v>
       </c>
       <c r="K51" t="n">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52">
@@ -2958,7 +2958,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -3045,13 +3045,13 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>646</v>
+        <v>984</v>
       </c>
       <c r="J53" t="n">
-        <v>10675</v>
+        <v>7129</v>
       </c>
       <c r="K53" t="n">
-        <v>2899</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="54">
@@ -3062,7 +3062,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -3094,13 +3094,13 @@
         </is>
       </c>
       <c r="I54" t="n">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="J54" t="n">
         <v>100</v>
       </c>
       <c r="K54" t="n">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55">
@@ -3111,7 +3111,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -3143,13 +3143,13 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>5376</v>
+        <v>6921</v>
       </c>
       <c r="J55" t="n">
-        <v>5669</v>
+        <v>19017</v>
       </c>
       <c r="K55" t="n">
-        <v>5525</v>
+        <v>16148</v>
       </c>
     </row>
     <row r="56">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>HANWASH - Master</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3192,13 +3192,13 @@
         </is>
       </c>
       <c r="I56" t="n">
-        <v>7859</v>
+        <v>1911</v>
       </c>
       <c r="J56" t="n">
-        <v>15348</v>
+        <v>19652</v>
       </c>
       <c r="K56" t="n">
-        <v>13865</v>
+        <v>3023</v>
       </c>
     </row>
     <row r="57">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -3247,7 +3247,7 @@
         <v>100</v>
       </c>
       <c r="K57" t="n">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="58">
@@ -3258,7 +3258,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -3290,13 +3290,13 @@
         </is>
       </c>
       <c r="I58" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="J58" t="n">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="K58" t="n">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59">
@@ -3307,7 +3307,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Mattson</t>
+          <t>Mattson LM</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -3339,13 +3339,13 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="J59" t="n">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K59" t="n">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
this version is preferred for now
</commit_message>
<xml_diff>
--- a/EDA/Hanwash_new_Indicators.xlsx
+++ b/EDA/Hanwash_new_Indicators.xlsx
@@ -627,7 +627,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>This indicator measures the level of engagement and support provided by Rotarians in WASH-related events in local communes, reflecting increased civil society engagement in WASH services.</t>
+          <t>Percentage of commune-level WASH events that have active Rotarian participation, measured as a proportion of total reported events.</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -636,13 +636,13 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="J4" t="n">
         <v>100</v>
       </c>
       <c r="K4" t="n">
-        <v>95</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5">
@@ -676,7 +676,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>The percentage of WASH events within communes that are led and coordinated by trained HANWASH Ambassadors and Coordinators, aiming to effectively communicate WASH messages and advocate for HANWASH goals. This reflects the level of leadership and initiative taken by trained personnel in promoting WASH activities.</t>
+          <t>Percentage of commune-level WASH events led by trained HANWASH Ambassadors and Coordinators to communicate WASH messages and advocate for HANWASH goals, measured as a proportion of total reported events.</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -685,13 +685,13 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="J5" t="n">
         <v>100</v>
       </c>
       <c r="K5" t="n">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6">
@@ -725,7 +725,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>The total number of hours that Rotarians volunteer each month participating in WASH initiatives and activities.</t>
+          <t>Average number of volunteer hours per month spent by Rotarians in WASH events, calculated per Rotary club.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -734,13 +734,13 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="J6" t="n">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="K6" t="n">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7">
@@ -774,7 +774,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>The total number of individuals who participate in or are impacted by WASH events and advocacy efforts led by HANWASH Ambassadors, Coordinators, and Rotarians. This indicates the outreach and engagement success of the WASH programs.</t>
+          <t>Total number of individuals reached through WASH events and advocacy efforts led by HANWASH Ambassadors, Coordinators, and Rotarians in the commune.</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -783,13 +783,13 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="J7" t="n">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="K7" t="n">
-        <v>78</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -823,7 +823,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>The total number of HANWASH Ambassadors who have successfully completed their training programs.</t>
+          <t>Total number of HANWASH Ambassadors who have successfully completed the required training program.</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -832,13 +832,13 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>18</v>
+        <v>88</v>
       </c>
       <c r="J8" t="n">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="K8" t="n">
-        <v>52</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9">
@@ -872,7 +872,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>The total number of HANWASH Coordinators who have successfully completed their training programs.</t>
+          <t>Total number of HANWASH Coordinators who have successfully completed the required training program.</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -881,13 +881,13 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="J9" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K9" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
@@ -921,7 +921,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The total count of educational and training materials developed that adhere to the three pillars and core values of HANWASH.</t>
+          <t>Number of training materials developed that align with HANWASH's three pillars and core values.</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -930,13 +930,13 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="K10" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -970,7 +970,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Number of hours and number of people attending</t>
+          <t>Cumulative number of training hours received by HANWASH Ambassadors, Coordinators, and their committees throughout the Caribbean region.</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -979,13 +979,13 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="J11" t="n">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="K11" t="n">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12">
@@ -1019,7 +1019,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The percentage of WASH interventions that have been approved and implemented in accordance with predefined Commune Action Plans, ensuring the initiatives are part of a strategic and coordinated approach to WASH improvements.</t>
+          <t>Percentage of implemented interventions that align with approved Commune Action Plans, indicating adherence to local priorities and needs.</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1028,13 +1028,13 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="J12" t="n">
         <v>100</v>
       </c>
       <c r="K12" t="n">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13">
@@ -1068,7 +1068,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>The number of communes that have developed action plans explicitly addressing water, sanitation, hygiene, and water resources management.</t>
+          <t>Number of communes with comprehensive action plans that explicitly address all four WASH aspects: Water, Sanitation, Hygiene, and Water Resources Management.</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1077,13 +1077,13 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="K13" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>The number of meetings and events held to plan and coordinate WASH activities involving DINEPA and municipal officials.</t>
+          <t>Number of WASH planning and coordination events conducted with DINEPA and municipal officials per month, fostering collaboration and alignment.</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -1126,13 +1126,13 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K14" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The percentage of service providers participating in the HANWASH initiative that are regularly monitored according to established national guidelines. This metric ensures that WASH service providers meet accountability standards, maintain quality service delivery, and uphold their responsibilities towards users as per national regulatory requirements.</t>
+          <t>Percentage of service providers under the HANWASH initiative that are monitored according to national guidelines, ensuring compliance and quality.</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1181,7 +1181,7 @@
         <v>100</v>
       </c>
       <c r="K15" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16">
@@ -1215,7 +1215,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>The percentage of service providers with established accountability mechanisms, such as regular meetings, community engagement, bylaws, fee collection, record-keeping, and monthly reporting to local authorities.</t>
+          <t>Percentage of intervention service providers that have established accountability structures, promoting transparency and community engagement.</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -1224,13 +1224,13 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="J16" t="n">
         <v>100</v>
       </c>
       <c r="K16" t="n">
-        <v>97</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17">
@@ -1264,7 +1264,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>This indicator measures the proportion of the households connected to the water system which are satisfied with the quality, affordability and reliability of the WASH services provided</t>
+          <t>Percentage of users expressing satisfaction with the quality, affordability, and reliability of WASH services provided, based on household surveys.</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1273,13 +1273,13 @@
         </is>
       </c>
       <c r="I17" t="n">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="J17" t="n">
         <v>100</v>
       </c>
       <c r="K17" t="n">
-        <v>96</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>The number of water systems within intervention areas that consistently submit monthly operational and performance reports, ensuring regular monitoring and transparency of water service delivery.</t>
+          <t>Number of intervention water systems that consistently report data on a regular basis, demonstrating operational transparency.</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1322,13 +1322,13 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J18" t="n">
         <v>3</v>
       </c>
       <c r="K18" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The percentage of customer complaints that are resolved within the same month they are identified.</t>
+          <t>Percentage of customer complaints resolved during the month, calculated as (number of resolved complaints / total number of complaints) * 100.</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1371,13 +1371,13 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>66</v>
+        <v>98</v>
       </c>
       <c r="J19" t="n">
         <v>100</v>
       </c>
       <c r="K19" t="n">
-        <v>76</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>This indicator measures how long it takes on average for the service providers to resolve customer complaints.</t>
+          <t>Average number of days taken to resolve customer complaints, indicating responsiveness and service quality.</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -1420,10 +1420,10 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="J20" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K20" t="n">
         <v>18</v>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>The percentage of water points in intervention areas that are operational (either fully functional or functional with minor repairs needed) and provide potable water, free from E. Coli and other priority contaminants, according to original design specifications.</t>
+          <t>Percentage of intervention water points that are both functioning and providing potable water, ensuring access to safe drinking water.</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -1522,13 +1522,13 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="J22" t="n">
         <v>100</v>
       </c>
       <c r="K22" t="n">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
@@ -1562,7 +1562,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>The percentage of people in intervention communes who have access to an improved water source within a 30-minute round trip, ensuring basic drinking water service at the household level.</t>
+          <t>Percentage of population in intervention communes with access to at least basic drinking water service, defined as an improved water source within 30 minutes round trip.</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1571,13 +1571,13 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="J23" t="n">
         <v>100</v>
       </c>
       <c r="K23" t="n">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24">
@@ -1611,7 +1611,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>The percentage of people in target areas who have access to safe drinking water that is always available, accessible at home, and free from contaminants.</t>
+          <t>Percentage of population in intervention communes with access to safely managed drinking water service, defined as an improved water source on premises, available when needed, and free from contamination.</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1620,13 +1620,13 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="J24" t="n">
         <v>100</v>
       </c>
       <c r="K24" t="n">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25">
@@ -1660,7 +1660,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>The percentage of water points in intervention areas that are fully operational, provide potable water, and maintain a balanced or surplus budget within two years from their inauguration date.</t>
+          <t>Percentage of intervention water points that are functioning, potable, and financially sustainable (balanced or surplus budget) after 2 years of operation.</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1669,13 +1669,13 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="J25" t="n">
         <v>100</v>
       </c>
       <c r="K25" t="n">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>The number of individuals in intervention communes who benefit from access to basic drinking water services provided by community-managed water points, ensuring sustainable and locally-managed water supply solutions.</t>
+          <t>Number of people in intervention communes gaining access to basic drinking water service through community-managed water points.</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -1718,13 +1718,13 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="J26" t="n">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K26" t="n">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>The total number of water points established and managed by local communities under DINEPA's guidelines.</t>
+          <t>Number of new community-managed water points created, with signed CPE statutes with DINEPA.</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1767,13 +1767,13 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="J27" t="n">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="K27" t="n">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
@@ -1807,7 +1807,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>The percentage of community-managed water points that submit monthly reports to local authorities.</t>
+          <t>Percentage of newly created community-managed water points that submit monthly reports to local authorities, promoting accountability.</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1816,13 +1816,13 @@
         </is>
       </c>
       <c r="I28" t="n">
+        <v>2</v>
+      </c>
+      <c r="J28" t="n">
+        <v>124</v>
+      </c>
+      <c r="K28" t="n">
         <v>119</v>
-      </c>
-      <c r="J28" t="n">
-        <v>136</v>
-      </c>
-      <c r="K28" t="n">
-        <v>124</v>
       </c>
     </row>
     <row r="29">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>The number of individuals who have gained access to safe drinking water through the project.</t>
+          <t>Number of people newly provided with safely managed drinking water service, meeting WHO/UNICEF Joint Monitoring Programme (JMP) criteria.</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1868,10 +1868,10 @@
         <v>4</v>
       </c>
       <c r="J29" t="n">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="K29" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>The number of existing piped water systems that have been restored to proper functionality in the target areas.</t>
+          <t>Number of professionally managed piped water systems rehabilitated in the intervention communes, improving existing infrastructure.</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1917,10 +1917,10 @@
         <v>1</v>
       </c>
       <c r="J30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>The number of new piped water systems established and professionally managed in the target areas.</t>
+          <t>Number of new professionally managed piped water systems created in the intervention communes, expanding water service coverage.</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>The percentage of communities in intervention areas that have been verified as Open Defecation Free by the commune WASH committee, meeting criteria such as the presence of usable toilets, no fecal matter in open areas, and willingness to maintain ODF status.</t>
+          <t>Percentage of intervention communities verified as Open Defecation Free (ODF), meeting all criteria set by the commune WASH committee.</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -2012,13 +2012,13 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="J32" t="n">
         <v>100</v>
       </c>
       <c r="K32" t="n">
-        <v>74</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t xml:space="preserve"> The percentage of people in intervention communes who have access to improved and unshared sanitation facilities, ensuring basic sanitation service at the household level.</t>
+          <t>Percentage of population in intervention communes with access to at least basic sanitation service, defined as improved and unshared facilities.</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -2061,13 +2061,13 @@
         </is>
       </c>
       <c r="I33" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J33" t="n">
         <v>100</v>
       </c>
       <c r="K33" t="n">
-        <v>77</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>The percentage of people in target areas who have access to safe, private (unshared) sanitation facilities where excreta are properly treated on-site or transported and treated off-site.</t>
+          <t>Percentage of population in intervention communes with access to safely managed sanitation service, meeting WHO/UNICEF JMP criteria.</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -2110,13 +2110,13 @@
         </is>
       </c>
       <c r="I34" t="n">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="J34" t="n">
         <v>100</v>
       </c>
       <c r="K34" t="n">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35">
@@ -2150,7 +2150,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>The number of individuals newly provided with access to basic sanitation services, including improved and unshared facilities, within intervention communes.</t>
+          <t>Number of people newly provided with access to basic sanitation service in the intervention communes.</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -2159,13 +2159,13 @@
         </is>
       </c>
       <c r="I35" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="J35" t="n">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="K35" t="n">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>The total number of communities in intervention areas that have achieved verification as Open Defecation Free, meeting the criteria set by the commune WASH committee.</t>
+          <t>Number of intervention communities that have been verified as Open Defecation Free (ODF) by the commune WASH committee.</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -2208,13 +2208,13 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>121</v>
+        <v>81</v>
       </c>
       <c r="J36" t="n">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="K36" t="n">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="37">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>The number of communities in intervention areas that have sustained Open Defecation Free status for at least one year and have been officially certified by the commune WASH committee.</t>
+          <t>Number of intervention communities that have been certified as Open Defecation Free (ODF), maintaining verified ODF status for at least one year.</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -2257,13 +2257,13 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>22</v>
+        <v>121</v>
       </c>
       <c r="J37" t="n">
-        <v>104</v>
+        <v>167</v>
       </c>
       <c r="K37" t="n">
-        <v>98</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Mattson LM</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>The number of public latrines built within the project scope.</t>
+          <t>Number of public latrines constructed, improving sanitation access in communal areas.</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -2306,13 +2306,13 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="J38" t="n">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="K38" t="n">
-        <v>122</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39">
@@ -2346,7 +2346,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>The percentage of people in intervention communes who have access to facilities with soap and water for handwashing, ensuring basic hygiene service at the household level.</t>
+          <t>Percentage of population in intervention communes with access to at least basic hygiene service, defined as presence of a handwashing facility with soap and water on premises.</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
@@ -2355,13 +2355,13 @@
         </is>
       </c>
       <c r="I39" t="n">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="J39" t="n">
         <v>100</v>
       </c>
       <c r="K39" t="n">
-        <v>68</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>The percentage of individuals newly provided with access to basic hygiene services, including handwashing facilities with soap and water within intervention communes.</t>
+          <t>Percentage of population in intervention communes with access to basic hygiene service, as defined by WHO/UNICEF JMP criteria.</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
@@ -2404,13 +2404,13 @@
         </is>
       </c>
       <c r="I40" t="n">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="J40" t="n">
         <v>100</v>
       </c>
       <c r="K40" t="n">
-        <v>53</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41">
@@ -2444,7 +2444,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>The total number of community animators who have completed training programs.</t>
+          <t>Number of community animators trained to provide hygiene education and community mobilization.</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -2453,13 +2453,13 @@
         </is>
       </c>
       <c r="I41" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J41" t="n">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="K41" t="n">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42">
@@ -2493,7 +2493,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>This indicator measures the intensity of the hygiene trainings and community mobilization  delivered by the community animators. It is the sum of hours the community animator spends providing hygiene trainings.</t>
+          <t>Cumulative number of hours of hygiene training and community mobilization provided by trained community animators.</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -2502,13 +2502,13 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J42" t="n">
-        <v>53</v>
+        <v>92</v>
       </c>
       <c r="K42" t="n">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43">
@@ -2542,7 +2542,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>The number of individuals newly provided with access to basic hygiene services, including handwashing facilities with soap and water within intervention communes.</t>
+          <t>Number of people newly provided with access to basic hygiene service in intervention areas.</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
@@ -2551,13 +2551,13 @@
         </is>
       </c>
       <c r="I43" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="J43" t="n">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="K43" t="n">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44">
@@ -2591,7 +2591,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>The percentage of schools in intervention areas that have improved, safe drinking water sources, functional sanitation facilities, and handwashing stations with soap and water.</t>
+          <t>Percentage of schools in intervention areas with basic drinking water, sanitation, and hygiene services, meeting WHO/UNICEF JMP criteria for schools.</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -2600,13 +2600,13 @@
         </is>
       </c>
       <c r="I44" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="J44" t="n">
         <v>100</v>
       </c>
       <c r="K44" t="n">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45">
@@ -2640,7 +2640,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>The percentage of healthcare facilities in intervention areas that have improved, safe drinking water sources, functioning sanitation facilities, and handwashing stations with soap and water or alcohol-based hand rubs. This metric ensures that healthcare facilities meet basic WASH standards.</t>
+          <t>Percentage of healthcare facilities in intervention areas with basic drinking water, sanitation, and hygiene services, meeting WHO/UNICEF JMP criteria for healthcare facilities.</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -2649,13 +2649,13 @@
         </is>
       </c>
       <c r="I45" t="n">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="J45" t="n">
         <v>100</v>
       </c>
       <c r="K45" t="n">
-        <v>73</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46">
@@ -2689,7 +2689,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>The total number of schools in intervention areas that have been provided with access to improved drinking water services, ensuring that they meet the required standards of water quality and availability.</t>
+          <t>Number of schools newly provided with basic drinking water services in intervention areas.</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -2698,13 +2698,13 @@
         </is>
       </c>
       <c r="I46" t="n">
-        <v>18</v>
+        <v>124</v>
       </c>
       <c r="J46" t="n">
-        <v>124</v>
+        <v>199</v>
       </c>
       <c r="K46" t="n">
-        <v>29</v>
+        <v>135</v>
       </c>
     </row>
     <row r="47">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>The total number of healthcare facilities in intervention areas that have been provided with access to improved drinking water services, ensuring safe and reliable water for patients and staff.</t>
+          <t>Number of healthcare facilities newly provided with basic drinking water services in intervention areas.</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
@@ -2747,13 +2747,13 @@
         </is>
       </c>
       <c r="I47" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J47" t="n">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="K47" t="n">
-        <v>52</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>The total number of schools in intervention areas that have been equipped with improved, functional sanitation facilities, including gender-separated and accessible toilets, to meet the needs of students and staff.</t>
+          <t>Number of schools newly provided with basic sanitation services in intervention areas.</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
@@ -2796,13 +2796,13 @@
         </is>
       </c>
       <c r="I48" t="n">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="J48" t="n">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="K48" t="n">
-        <v>170</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>The total number of healthcare facilities in intervention areas that have been equipped with improved, functional sanitation facilities, including dedicated and accessible toilets. These facilities are designed to meet the sanitation needs of all healthcare users.</t>
+          <t>Number of healthcare facilities newly provided with basic sanitation services in intervention areas.</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -2845,13 +2845,13 @@
         </is>
       </c>
       <c r="I49" t="n">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="J49" t="n">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K49" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>The total number of schools in intervention areas that have been provided with handwashing facilities, including soap and water, ensuring basic hygiene practices are accessible to all students and staff.</t>
+          <t>Number of schools newly provided with basic hygiene services in intervention areas.</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -2894,13 +2894,13 @@
         </is>
       </c>
       <c r="I50" t="n">
-        <v>98</v>
+        <v>149</v>
       </c>
       <c r="J50" t="n">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="K50" t="n">
-        <v>102</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51">
@@ -2934,7 +2934,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>The total number of healthcare facilities in intervention areas that have been provided with handwashing facilities, including soap and water or alcohol-based hand rubs, ensuring basic hygiene practices are accessible to all patients and staff.</t>
+          <t>Number of healthcare facilities newly provided with basic hygiene services in intervention areas.</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -2943,13 +2943,13 @@
         </is>
       </c>
       <c r="I51" t="n">
-        <v>50</v>
+        <v>154</v>
       </c>
       <c r="J51" t="n">
-        <v>157</v>
+        <v>198</v>
       </c>
       <c r="K51" t="n">
-        <v>111</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52">
@@ -3036,7 +3036,7 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>The total amount of funds pledged by stakeholders in accordance with HANWASH Core Values.</t>
+          <t>Cumulative amount of money (in USD) committed to projects aligned with HANWASH Core Values, including local leadership, collaboration, systematic approach, impact, and commitment.</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
@@ -3045,13 +3045,13 @@
         </is>
       </c>
       <c r="I53" t="n">
-        <v>984</v>
+        <v>2673</v>
       </c>
       <c r="J53" t="n">
-        <v>7129</v>
+        <v>6610</v>
       </c>
       <c r="K53" t="n">
-        <v>2605</v>
+        <v>6130</v>
       </c>
     </row>
     <row r="54">
@@ -3085,7 +3085,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>The cumulative percentage of allocated funds that have been spent over the project duration. This metric is calculated by dividing the total amount spent by the total committed funds and multiplying by 100, reflecting the financial resource utilization efficiency of the project.</t>
+          <t>Percentage of committed funds that have been spent, calculated as (Cumulative_amount_spent / Cumulative_amount_committed) * 100.</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
@@ -3094,13 +3094,13 @@
         </is>
       </c>
       <c r="I54" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="J54" t="n">
         <v>100</v>
       </c>
       <c r="K54" t="n">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="55">
@@ -3134,7 +3134,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>The total amount of money spent by external organizations or entities within the areas covered by HANWASH projects.</t>
+          <t>Amount of money (in USD) spent by external actors within HANWASH project areas, aligned with HANWASH Core Values.</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
@@ -3143,13 +3143,13 @@
         </is>
       </c>
       <c r="I55" t="n">
-        <v>6921</v>
+        <v>6666</v>
       </c>
       <c r="J55" t="n">
-        <v>19017</v>
+        <v>6717</v>
       </c>
       <c r="K55" t="n">
-        <v>16148</v>
+        <v>6714</v>
       </c>
     </row>
     <row r="56">
@@ -3160,7 +3160,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Mattson LM</t>
+          <t>HANWASH-Master LM</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -3183,7 +3183,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>The total amount of money spent by external entities outside the HANWASH project areas, in line with HANWASH Core Values.</t>
+          <t>Amount of money (in USD) spent by external actors beyond HANWASH project areas but still aligned with HANWASH Core Values, extending impact.</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
@@ -3192,13 +3192,13 @@
         </is>
       </c>
       <c r="I56" t="n">
-        <v>1911</v>
+        <v>592</v>
       </c>
       <c r="J56" t="n">
-        <v>19652</v>
+        <v>18525</v>
       </c>
       <c r="K56" t="n">
-        <v>3023</v>
+        <v>16246</v>
       </c>
     </row>
     <row r="57">
@@ -3232,7 +3232,7 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Number of IPs who have signed  Total number of IPs in HANWASH program areas x 100</t>
+          <t>Percentage of implementing partners in HANWASH program areas who have signed the DINEPA Accord Cadre, ensuring alignment with national standards.</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -3241,13 +3241,13 @@
         </is>
       </c>
       <c r="I57" t="n">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="J57" t="n">
         <v>100</v>
       </c>
       <c r="K57" t="n">
-        <v>89</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>The total number of DINEPA personnel who have undergone leadership training programs.</t>
+          <t>Number of DINEPA personnel who have completed leadership training, building capacity within the national water authority.</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
@@ -3290,13 +3290,13 @@
         </is>
       </c>
       <c r="I58" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J58" t="n">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="K58" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -3330,7 +3330,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>The number of technical training sessions delivered to address DINEPA's prioritized areas, including the unified national tariff methodology and ODF certification for 2023-24.</t>
+          <t>Number of technical trainings provided for DINEPA priority areas, focusing on key topics such as unified national tariff methodology and ODF certification.</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
@@ -3339,13 +3339,13 @@
         </is>
       </c>
       <c r="I59" t="n">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="J59" t="n">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="K59" t="n">
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>